<commit_message>
Drop in US files
</commit_message>
<xml_diff>
--- a/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
+++ b/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junshepard/Library/Containers/com.microsoft.Excel/Data/state-eps-data-repository/template_state/trans/TTLE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\TTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF038AB-6E90-6345-83FC-B41548C707B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38156F0C-A178-4103-B28F-F0C9E7C7D60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -102,7 +102,7 @@
     <numFmt numFmtId="164" formatCode="###0.00_)"/>
     <numFmt numFmtId="165" formatCode="#,##0_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -767,7 +767,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -779,7 +779,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="60">
     <cellStyle name="20% - Accent1" xfId="33" builtinId="30" customBuiltin="1"/>
@@ -1207,26 +1206,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="45.5" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="7">
-        <v>44308</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1234,194 +1228,194 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="2:2" s="2" customFormat="1"/>
-    <row r="24" spans="2:2" s="2" customFormat="1"/>
-    <row r="25" spans="2:2" s="2" customFormat="1"/>
-    <row r="26" spans="2:2" s="2" customFormat="1"/>
-    <row r="27" spans="2:2" s="2" customFormat="1"/>
-    <row r="28" spans="2:2" s="2" customFormat="1"/>
-    <row r="29" spans="2:2">
+    <row r="23" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="2:2">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="2:2">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="2:2">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="2:2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="2:2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="2:2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="2:2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="2:2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="2:2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="2:2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="2:2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="2:2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="2:2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="2:2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="2:2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B62" s="2"/>
     </row>
   </sheetData>
@@ -1437,16 +1431,18 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -1457,18 +1453,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>-3</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="2">
         <v>-3</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1479,7 +1475,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1490,7 +1486,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1501,7 +1497,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1512,7 +1508,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Revert "Drop in US files"
This reverts commit 57ab2f619a3d27c002cc315f97df0c04452473ce.
</commit_message>
<xml_diff>
--- a/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
+++ b/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\TTLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junshepard/Library/Containers/com.microsoft.Excel/Data/state-eps-data-repository/template_state/trans/TTLE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38156F0C-A178-4103-B28F-F0C9E7C7D60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF038AB-6E90-6345-83FC-B41548C707B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -102,7 +102,7 @@
     <numFmt numFmtId="164" formatCode="###0.00_)"/>
     <numFmt numFmtId="165" formatCode="#,##0_)"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -767,7 +767,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -779,6 +779,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="60">
     <cellStyle name="20% - Accent1" xfId="33" builtinId="30" customBuiltin="1"/>
@@ -1206,21 +1207,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="45.453125" customWidth="1"/>
+    <col min="2" max="2" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="7">
+        <v>44308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1228,194 +1234,194 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:2">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" s="2" customFormat="1"/>
+    <row r="24" spans="2:2" s="2" customFormat="1"/>
+    <row r="25" spans="2:2" s="2" customFormat="1"/>
+    <row r="26" spans="2:2" s="2" customFormat="1"/>
+    <row r="27" spans="2:2" s="2" customFormat="1"/>
+    <row r="28" spans="2:2" s="2" customFormat="1"/>
+    <row r="29" spans="2:2">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:2">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:2">
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:2">
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2">
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2">
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2">
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2">
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2">
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2">
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2">
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2">
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:2">
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:2">
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2">
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:2">
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:2">
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:2">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:2">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:2">
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2">
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2">
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2">
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2">
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2">
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2">
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2">
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2">
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2">
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2">
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2">
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2">
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2">
       <c r="B62" s="2"/>
     </row>
   </sheetData>
@@ -1431,18 +1437,16 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -1453,18 +1457,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>-3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4">
         <v>-3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1475,7 +1479,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1486,7 +1490,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1497,7 +1501,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1508,7 +1512,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>6</v>
       </c>

</xml_diff>